<commit_message>
Changes to LER calculation
</commit_message>
<xml_diff>
--- a/DATA/LER/PV_PANEL_DATA.xlsx
+++ b/DATA/LER/PV_PANEL_DATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au759124_uni_au_dk/Documents/Documents/V4F_agrivoltaics/DATA/PV_DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{9E4825C6-CA3E-420A-B195-074792FA7909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3935DFD9-2F59-49A9-8011-D4996D18AC78}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{9E4825C6-CA3E-420A-B195-074792FA7909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EF9AC22-67AE-46BA-8B31-9B60B0A7B479}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="4395" windowWidth="21600" windowHeight="12645" xr2:uid="{FF9333E0-2E62-4BF0-AD5B-84AA6DC9364F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF9333E0-2E62-4BF0-AD5B-84AA6DC9364F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>PV_SETUP</t>
   </si>
   <si>
-    <t>SOUTH-ORIENTED</t>
-  </si>
-  <si>
     <t>VERTICAL</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>EFFECIENCY_KWH_KW</t>
+  </si>
+  <si>
+    <t>SOUTH_ORIENTED</t>
   </si>
 </sst>
 </file>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA55AACC-BFEE-42FA-A1FE-DA8675B96993}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,33 +508,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
         <v>0.2</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>0.2</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3">
         <v>0.5</v>

</xml_diff>